<commit_message>
Glossary : kunde og bruger tilføjet + featureliste : brugerprofil
</commit_message>
<xml_diff>
--- a/Analysis/Glossary.xlsx
+++ b/Analysis/Glossary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juyoung Choi\Desktop\1stYear Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juyoung Choi\iCloudDrive\eclipse\flextur\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Glossary</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Aliases</t>
   </si>
   <si>
-    <t>Midt trafik</t>
-  </si>
-  <si>
     <t>pengeinstitut</t>
   </si>
   <si>
@@ -88,6 +85,30 @@
   </si>
   <si>
     <t>profil</t>
+  </si>
+  <si>
+    <t>Inception draft 2</t>
+  </si>
+  <si>
+    <t>3.maj 2016</t>
+  </si>
+  <si>
+    <t>MidtTrafik</t>
+  </si>
+  <si>
+    <t>kunde</t>
+  </si>
+  <si>
+    <t>bruger</t>
+  </si>
+  <si>
+    <t>dem der anvender systemet til at bestille flextur</t>
+  </si>
+  <si>
+    <t>dem der bestiller og anvender systemet</t>
+  </si>
+  <si>
+    <t>MidtTrafik og bruger aliases tilføjet</t>
   </si>
 </sst>
 </file>
@@ -147,20 +168,50 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -187,14 +238,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:E16" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:E16" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <autoFilter ref="A3:E16"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Term"/>
-    <tableColumn id="2" name="Definition and information"/>
-    <tableColumn id="3" name="Format"/>
-    <tableColumn id="4" name="Validation Rules"/>
-    <tableColumn id="5" name="Aliases"/>
+    <tableColumn id="1" name="Term" dataDxfId="6"/>
+    <tableColumn id="2" name="Definition and information" dataDxfId="0"/>
+    <tableColumn id="3" name="Format" dataDxfId="5"/>
+    <tableColumn id="4" name="Validation Rules" dataDxfId="4"/>
+    <tableColumn id="5" name="Aliases" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -463,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,20 +529,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -518,6 +569,20 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -539,72 +604,86 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E9" s="3"/>
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Glossary, Usecase liste added
</commit_message>
<xml_diff>
--- a/Analysis/Glossary.xlsx
+++ b/Analysis/Glossary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Revision list" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
   <si>
     <t>Glossary</t>
   </si>
@@ -175,6 +175,30 @@
   </si>
   <si>
     <t>login, profil, id, kodeord tilføjet</t>
+  </si>
+  <si>
+    <t>4.maj 2016</t>
+  </si>
+  <si>
+    <t>Inception draft 5</t>
+  </si>
+  <si>
+    <t>MidtTrafiks medarbejder</t>
+  </si>
+  <si>
+    <t>kunde til MidtTrafiks kunde, MidtTrafiks medarbejder til bestillingsmodtagelse</t>
+  </si>
+  <si>
+    <t>Inception draft 6</t>
+  </si>
+  <si>
+    <t>historik = turhistorik</t>
+  </si>
+  <si>
+    <t>historik</t>
+  </si>
+  <si>
+    <t>turhistorik</t>
   </si>
 </sst>
 </file>
@@ -247,12 +271,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -262,10 +280,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -283,13 +307,13 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -321,14 +345,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:E15" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:E15" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A3:E15"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Term" dataDxfId="6"/>
-    <tableColumn id="2" name="Definition and information" dataDxfId="5"/>
-    <tableColumn id="3" name="Format" dataDxfId="4"/>
-    <tableColumn id="4" name="Validation Rules" dataDxfId="3"/>
-    <tableColumn id="5" name="Aliases" dataDxfId="2"/>
+    <tableColumn id="1" name="Term" dataDxfId="4"/>
+    <tableColumn id="2" name="Definition and information" dataDxfId="3"/>
+    <tableColumn id="3" name="Format" dataDxfId="2"/>
+    <tableColumn id="4" name="Validation Rules" dataDxfId="1"/>
+    <tableColumn id="5" name="Aliases" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -597,35 +621,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.109375" customWidth="1"/>
-    <col min="3" max="3" width="44.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -694,6 +718,34 @@
         <v>49</v>
       </c>
       <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" t="s">
         <v>7</v>
       </c>
     </row>
@@ -712,81 +764,81 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="5"/>
+    <col min="3" max="3" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -794,34 +846,37 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="E9" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -829,7 +884,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -837,25 +892,33 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FS-UC3 tilføjet : needs to check and match to mockups and glossary
</commit_message>
<xml_diff>
--- a/Analysis/Glossary.xlsx
+++ b/Analysis/Glossary.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t>Glossary</t>
   </si>
@@ -199,6 +199,15 @@
   </si>
   <si>
     <t>turhistorik</t>
+  </si>
+  <si>
+    <t>bruger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bruger til systemet (ubestemt role) </t>
+  </si>
+  <si>
+    <t>(kunden og bestillingesmodtagelse)</t>
   </si>
 </sst>
 </file>
@@ -266,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -278,6 +287,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -345,8 +357,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:E15" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A3:E15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:E16" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A3:E16"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Term" dataDxfId="4"/>
     <tableColumn id="2" name="Definition and information" dataDxfId="3"/>
@@ -636,20 +648,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -764,10 +776,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,13 +794,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -919,6 +931,19 @@
       </c>
       <c r="E15" s="2" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UC2 ekstra tilbehør + pris
</commit_message>
<xml_diff>
--- a/Analysis/Glossary.xlsx
+++ b/Analysis/Glossary.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
   <si>
     <t>Glossary</t>
   </si>
@@ -208,6 +208,15 @@
   </si>
   <si>
     <t>mindst 6 bogstav eller cpr-nummer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> antal af bagage, barnevogne eller autostole, samt behov for hjælpemidler - SF-UC2-bestilFlextur</t>
+  </si>
+  <si>
+    <t>ikke-obligatorisk oplsyninger</t>
+  </si>
+  <si>
+    <t>ekstra tilbehør</t>
   </si>
 </sst>
 </file>
@@ -275,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -287,6 +296,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -357,8 +369,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:E16" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A3:E16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:E43" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A3:E43"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Term" dataDxfId="4"/>
     <tableColumn id="2" name="Definition and information" dataDxfId="3"/>
@@ -648,20 +660,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -776,10 +788,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D14" sqref="D13:D14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -794,13 +806,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -945,6 +957,175 @@
       <c r="E16" s="5" t="s">
         <v>59</v>
       </c>
+    </row>
+    <row r="17" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Glossary, UC2-TC, UC3-TC tilføjet
</commit_message>
<xml_diff>
--- a/Analysis/Glossary.xlsx
+++ b/Analysis/Glossary.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
   <si>
     <t>Glossary</t>
   </si>
@@ -105,9 +105,6 @@
     <t>.jar</t>
   </si>
   <si>
-    <t>MidtTrafik virksomhed</t>
-  </si>
-  <si>
     <t>flextur_sats.jar</t>
   </si>
   <si>
@@ -204,19 +201,58 @@
     <t xml:space="preserve">bruger til systemet (ubestemt role) </t>
   </si>
   <si>
-    <t>(kunden og bestillingesmodtagelse)</t>
-  </si>
-  <si>
     <t>mindst 6 bogstav eller cpr-nummer</t>
   </si>
   <si>
-    <t xml:space="preserve"> antal af bagage, barnevogne eller autostole, samt behov for hjælpemidler - SF-UC2-bestilFlextur</t>
-  </si>
-  <si>
     <t>ikke-obligatorisk oplsyninger</t>
   </si>
   <si>
     <t>ekstra tilbehør</t>
+  </si>
+  <si>
+    <t>ugyldig dato</t>
+  </si>
+  <si>
+    <t>tjek date.now() /LocalDate.now()</t>
+  </si>
+  <si>
+    <t>SF-UC2-bestilFlextur</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> antal af bagage, barnevogne eller autostole, samt behov for hjælpemidler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dato der ikke er kommende dag ( ligger i datid) </t>
+  </si>
+  <si>
+    <t>Specifik UC reference</t>
+  </si>
+  <si>
+    <t>Inception draft 7</t>
+  </si>
+  <si>
+    <t>10.maj 2016</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>MidtTrafik virksomhed, Chef af MidtTrafik</t>
+  </si>
+  <si>
+    <t>13-15 tilføjet</t>
+  </si>
+  <si>
+    <t>Inception draft 8</t>
+  </si>
+  <si>
+    <t>9.maj 2016</t>
+  </si>
+  <si>
+    <t>bruger ( kunde eller bestillingsmodtagelse)</t>
+  </si>
+  <si>
+    <t>(kunden eller bestillingesmodtagelse)</t>
   </si>
 </sst>
 </file>
@@ -284,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -296,6 +332,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -320,7 +359,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="9">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -356,8 +401,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:D14" totalsRowShown="0">
-  <autoFilter ref="A5:D14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:D15" totalsRowShown="0">
+  <autoFilter ref="A5:D15"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Version"/>
     <tableColumn id="2" name="Date"/>
@@ -369,14 +414,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:E43" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A3:E43"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Term" dataDxfId="4"/>
-    <tableColumn id="2" name="Definition and information" dataDxfId="3"/>
-    <tableColumn id="3" name="Format" dataDxfId="2"/>
-    <tableColumn id="4" name="Validation Rules" dataDxfId="1"/>
-    <tableColumn id="5" name="Aliases" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:G43" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A3:G43"/>
+  <tableColumns count="7">
+    <tableColumn id="7" name="ID" dataDxfId="0"/>
+    <tableColumn id="1" name="Term" dataDxfId="6"/>
+    <tableColumn id="2" name="Definition and information" dataDxfId="5"/>
+    <tableColumn id="6" name="Specifik UC reference" dataDxfId="1"/>
+    <tableColumn id="3" name="Format" dataDxfId="4"/>
+    <tableColumn id="4" name="Validation Rules" dataDxfId="3"/>
+    <tableColumn id="5" name="Aliases" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -645,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,20 +707,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -719,13 +766,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -733,13 +780,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -747,13 +794,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -761,15 +808,43 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
         <v>53</v>
       </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>54</v>
-      </c>
       <c r="D11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" t="s">
         <v>7</v>
       </c>
     </row>
@@ -788,344 +863,518 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.109375" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="3"/>
+    <col min="7" max="7" width="11.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>13</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
+        <v>14</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="B18" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6" t="s">
+      <c r="E18" s="6"/>
+      <c r="F18" s="6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
       <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
       <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
       <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
       <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
       <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
       <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
       <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
       <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="7"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
       <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="7"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
       <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
       <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
       <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
       <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
       <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
       <c r="E33" s="6"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
       <c r="E34" s="6"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
       <c r="E35" s="6"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
       <c r="E36" s="6"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
       <c r="E37" s="6"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
       <c r="E38" s="6"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
       <c r="E39" s="6"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
       <c r="E40" s="6"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
       <c r="E41" s="6"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="7"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
       <c r="E42" s="6"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
       <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>